<commit_message>
Completed the Function Import with all Test green. - (Task #966)
Put your Message here.

---
Task #966: Add CostTypeExportWizard
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ElementDefinitionTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ElementDefinitionTest.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.budget.cost.test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A957E34-A167-458D-BDC5-4847F3BCFB62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="105" windowWidth="20115" windowHeight="9525"/>
+    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
-    <sheet name="InterfaceTypes" sheetId="8" r:id="rId2"/>
-    <sheet name="InterfaceEnds" sheetId="9" r:id="rId3"/>
-    <sheet name="Interfaces" sheetId="5" r:id="rId4"/>
+    <sheet name="CostTypes" sheetId="8" r:id="rId2"/>
+    <sheet name="CostEquipments" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t xml:space="preserve"> Structural Element UUID</t>
   </si>
@@ -67,39 +72,9 @@
     <t>UUID</t>
   </si>
   <si>
-    <t>VirSat IO Sheet for InterfaceEnds</t>
-  </si>
-  <si>
-    <t>Interface Type</t>
-  </si>
-  <si>
-    <t>InterfaceEnd Name</t>
-  </si>
-  <si>
-    <t>Interface Type Name</t>
-  </si>
-  <si>
-    <t>VirSat IO Sheet for Interface Types</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Interface Name</t>
-  </si>
-  <si>
-    <t>VirSat IO Sheet for Interfaces</t>
-  </si>
-  <si>
     <t>74ccc93a-281b-4ab8-ace4-cb7f2b9827d4b</t>
   </si>
   <si>
-    <t>BATTERY1</t>
-  </si>
-  <si>
     <t>supe_us</t>
   </si>
   <si>
@@ -112,31 +87,49 @@
     <t>POW_IN</t>
   </si>
   <si>
-    <t>HILL</t>
-  </si>
-  <si>
     <t>9f8b18e1-f6a1-4cf6-bcb7-0d4a5f0a86de</t>
   </si>
   <si>
     <t>POW_SOMETHING</t>
   </si>
   <si>
-    <t>BILL</t>
-  </si>
-  <si>
     <t>e13ad850-21d8-43d7-aa61-20a3f8d1749b</t>
   </si>
   <si>
     <t>POW_OUT</t>
   </si>
   <si>
-    <t>KILL</t>
+    <t>BIII</t>
+  </si>
+  <si>
+    <t>BAAA</t>
+  </si>
+  <si>
+    <t>BUUU</t>
+  </si>
+  <si>
+    <t>VirSat IO Sheet for Cost Types</t>
+  </si>
+  <si>
+    <t>Cost Type Name</t>
+  </si>
+  <si>
+    <t>VirSat IO Sheet for CostEquipments</t>
+  </si>
+  <si>
+    <t>Cost Type</t>
+  </si>
+  <si>
+    <t>CostEquipment Name</t>
+  </si>
+  <si>
+    <t>BATTERY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -416,9 +409,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -450,14 +440,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -495,9 +488,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,9 +523,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -565,9 +575,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -740,42 +767,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
+    <row r="1" spans="1:3" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="14"/>
     </row>
-    <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:3" ht="128.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="1:3" ht="128.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="23"/>
-    </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="22"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -786,89 +813,89 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -883,42 +910,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-    </row>
-    <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="1:3" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="1:3" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20"/>
-    </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="19"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
@@ -926,18 +953,18 @@
         <v>14</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="24"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -952,46 +979,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="1:4" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="1:4" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
@@ -999,69 +1026,69 @@
         <v>14</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1">
         <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="24"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1073,90 +1100,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-    </row>
-    <row r="3" spans="1:5" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed unpassed ImportValidatorTest - (Task #967)
---
Task #967: Add CostEquipmentWizard
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ElementDefinitionTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ElementDefinitionTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.budget.cost.test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A957E34-A167-458D-BDC5-4847F3BCFB62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E912060F-E968-4BF6-A0AC-4CD48DE82054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t xml:space="preserve"> Structural Element UUID</t>
   </si>
@@ -84,30 +84,12 @@
     <t>a2643ddb-e6a1-4015-9b80-be931f330c5a37</t>
   </si>
   <si>
-    <t>POW_IN</t>
-  </si>
-  <si>
     <t>9f8b18e1-f6a1-4cf6-bcb7-0d4a5f0a86de</t>
   </si>
   <si>
-    <t>POW_SOMETHING</t>
-  </si>
-  <si>
     <t>e13ad850-21d8-43d7-aa61-20a3f8d1749b</t>
   </si>
   <si>
-    <t>POW_OUT</t>
-  </si>
-  <si>
-    <t>BIII</t>
-  </si>
-  <si>
-    <t>BAAA</t>
-  </si>
-  <si>
-    <t>BUUU</t>
-  </si>
-  <si>
     <t>VirSat IO Sheet for Cost Types</t>
   </si>
   <si>
@@ -123,7 +105,28 @@
     <t>CostEquipment Name</t>
   </si>
   <si>
-    <t>BATTERY</t>
+    <t>CostMaterial</t>
+  </si>
+  <si>
+    <t>CostPersonal</t>
+  </si>
+  <si>
+    <t>CostTest</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>BATTERY_1</t>
+  </si>
+  <si>
+    <t>Entwicklung</t>
+  </si>
+  <si>
+    <t>Material</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -827,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -914,7 +917,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,7 +934,7 @@
     </row>
     <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -953,7 +956,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -982,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,7 +1005,7 @@
     </row>
     <row r="2" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1026,10 +1029,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1038,51 +1041,51 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
-        <v>1</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed import test cases - Task #967
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ElementDefinitionTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ElementDefinitionTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.budget.cost.test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A957E34-A167-458D-BDC5-4847F3BCFB62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ABB73A-39F6-4A2F-9824-A7122E74289E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -84,30 +84,12 @@
     <t>a2643ddb-e6a1-4015-9b80-be931f330c5a37</t>
   </si>
   <si>
-    <t>POW_IN</t>
-  </si>
-  <si>
     <t>9f8b18e1-f6a1-4cf6-bcb7-0d4a5f0a86de</t>
   </si>
   <si>
-    <t>POW_SOMETHING</t>
-  </si>
-  <si>
     <t>e13ad850-21d8-43d7-aa61-20a3f8d1749b</t>
   </si>
   <si>
-    <t>POW_OUT</t>
-  </si>
-  <si>
-    <t>BIII</t>
-  </si>
-  <si>
-    <t>BAAA</t>
-  </si>
-  <si>
-    <t>BUUU</t>
-  </si>
-  <si>
     <t>VirSat IO Sheet for Cost Types</t>
   </si>
   <si>
@@ -123,7 +105,25 @@
     <t>CostEquipment Name</t>
   </si>
   <si>
-    <t>BATTERY</t>
+    <t>CostMaterial</t>
+  </si>
+  <si>
+    <t>CostPersonal</t>
+  </si>
+  <si>
+    <t>CostTest</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>BATTERY_1</t>
+  </si>
+  <si>
+    <t>Entwicklung</t>
+  </si>
+  <si>
+    <t>Material</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -914,7 +914,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,7 +931,7 @@
     </row>
     <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -953,7 +953,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="2" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1026,10 +1026,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1038,51 +1038,51 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>